<commit_message>
Grensejustering Risør og Tvedestrand
</commit_message>
<xml_diff>
--- a/kostraleveranse2024/Kostra 01 - Vegnett hele landet.xlsx
+++ b/kostraleveranse2024/Kostra 01 - Vegnett hele landet.xlsx
@@ -6937,22 +6937,22 @@
         <v>4201</v>
       </c>
       <c r="C214" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D214" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E214" t="n">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="F214" t="n">
         <v>0</v>
       </c>
       <c r="G214" t="n">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H214" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="215">
@@ -7171,22 +7171,22 @@
         <v>4213</v>
       </c>
       <c r="C223" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D223" t="n">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E223" t="n">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F223" t="n">
         <v>0</v>
       </c>
       <c r="G223" t="n">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H223" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="224">
@@ -14456,7 +14456,7 @@
         <v>4201</v>
       </c>
       <c r="C214" t="n">
-        <v>428.1301190000011</v>
+        <v>444.1075360000013</v>
       </c>
     </row>
     <row r="215">
@@ -14555,7 +14555,7 @@
         <v>4213</v>
       </c>
       <c r="C223" t="n">
-        <v>478.0068830000001</v>
+        <v>462.0294660000001</v>
       </c>
     </row>
     <row r="224">
@@ -32183,7 +32183,7 @@
         </is>
       </c>
       <c r="D1007" t="n">
-        <v>8.699129000000001</v>
+        <v>11.053989</v>
       </c>
     </row>
     <row r="1008">
@@ -32199,7 +32199,7 @@
         </is>
       </c>
       <c r="D1008" t="n">
-        <v>90.09816800000002</v>
+        <v>93.09796400000002</v>
       </c>
     </row>
     <row r="1009">
@@ -32215,7 +32215,7 @@
         </is>
       </c>
       <c r="D1009" t="n">
-        <v>65.24244500000005</v>
+        <v>67.27543600000004</v>
       </c>
     </row>
     <row r="1010">
@@ -32231,7 +32231,7 @@
         </is>
       </c>
       <c r="D1010" t="n">
-        <v>171.8480380000001</v>
+        <v>176.9919570000001</v>
       </c>
     </row>
     <row r="1011">
@@ -32247,7 +32247,7 @@
         </is>
       </c>
       <c r="D1011" t="n">
-        <v>92.24233900000002</v>
+        <v>95.68819000000002</v>
       </c>
     </row>
     <row r="1012">
@@ -32887,7 +32887,7 @@
         </is>
       </c>
       <c r="D1051" t="n">
-        <v>24.97769800000001</v>
+        <v>22.62283800000001</v>
       </c>
     </row>
     <row r="1052">
@@ -32903,7 +32903,7 @@
         </is>
       </c>
       <c r="D1052" t="n">
-        <v>114.982331</v>
+        <v>111.982535</v>
       </c>
     </row>
     <row r="1053">
@@ -32919,7 +32919,7 @@
         </is>
       </c>
       <c r="D1053" t="n">
-        <v>56.70186100000004</v>
+        <v>54.66887000000006</v>
       </c>
     </row>
     <row r="1054">
@@ -32935,7 +32935,7 @@
         </is>
       </c>
       <c r="D1054" t="n">
-        <v>172.0318390000003</v>
+        <v>166.8879200000004</v>
       </c>
     </row>
     <row r="1055">
@@ -32951,7 +32951,7 @@
         </is>
       </c>
       <c r="D1055" t="n">
-        <v>109.3131539999999</v>
+        <v>105.8673029999999</v>
       </c>
     </row>
     <row r="1056">
@@ -42833,7 +42833,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2025-01-13</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Siste kvalitetssikring grensejustering Risør
</commit_message>
<xml_diff>
--- a/kostraleveranse2024/Kostra 01 - Vegnett hele landet.xlsx
+++ b/kostraleveranse2024/Kostra 01 - Vegnett hele landet.xlsx
@@ -14456,7 +14456,7 @@
         <v>4201</v>
       </c>
       <c r="C214" t="n">
-        <v>444.1075360000013</v>
+        <v>444.1339360000013</v>
       </c>
     </row>
     <row r="215">
@@ -14555,7 +14555,7 @@
         <v>4213</v>
       </c>
       <c r="C223" t="n">
-        <v>462.0294660000001</v>
+        <v>462.0030660000001</v>
       </c>
     </row>
     <row r="224">
@@ -32231,7 +32231,7 @@
         </is>
       </c>
       <c r="D1010" t="n">
-        <v>176.9919570000001</v>
+        <v>177.0183570000001</v>
       </c>
     </row>
     <row r="1011">
@@ -32935,7 +32935,7 @@
         </is>
       </c>
       <c r="D1054" t="n">
-        <v>166.8879200000004</v>
+        <v>166.8615200000004</v>
       </c>
     </row>
     <row r="1055">

</xml_diff>